<commit_message>
integration, preparation of charts for cnn
</commit_message>
<xml_diff>
--- a/cnn/benchmark_results/AAPL.xlsx
+++ b/cnn/benchmark_results/AAPL.xlsx
@@ -488,28 +488,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002775119617225144</v>
+        <v>0.2655023923444979</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001026915681026913</v>
+        <v>0.1780314964237858</v>
       </c>
       <c r="E2" t="n">
-        <v>2.15311004784689</v>
+        <v>19.61722488038277</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="G2" t="n">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="H2" t="n">
-        <v>97.84688995215312</v>
+        <v>80.38277511961722</v>
       </c>
       <c r="I2" t="n">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -520,28 +520,28 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.03763157894736819</v>
+        <v>0.4253349282296651</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.03259478300136334</v>
+        <v>0.2816908527697883</v>
       </c>
       <c r="E3" t="n">
-        <v>2.15311004784689</v>
+        <v>16.74641148325359</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="G3" t="n">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="H3" t="n">
-        <v>97.84688995215312</v>
+        <v>83.25358851674642</v>
       </c>
       <c r="I3" t="n">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -552,28 +552,28 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1155263157894735</v>
+        <v>0.6993540669856464</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.09195194766562532</v>
+        <v>0.4665462388390477</v>
       </c>
       <c r="E4" t="n">
-        <v>2.392344497607656</v>
+        <v>22.2488038277512</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="G4" t="n">
-        <v>216</v>
+        <v>158</v>
       </c>
       <c r="H4" t="n">
-        <v>97.60765550239235</v>
+        <v>77.75119617224881</v>
       </c>
       <c r="I4" t="n">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -584,28 +584,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1058133971291864</v>
+        <v>0.8397846889952156</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.08369526267999232</v>
+        <v>0.5670691775909864</v>
       </c>
       <c r="E5" t="n">
-        <v>2.631578947368421</v>
+        <v>22.96650717703349</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="G5" t="n">
-        <v>217</v>
+        <v>161</v>
       </c>
       <c r="H5" t="n">
-        <v>97.36842105263158</v>
+        <v>77.03349282296651</v>
       </c>
       <c r="I5" t="n">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -616,28 +616,28 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.1466028708133971</v>
+        <v>1.038181818181819</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1123804132629857</v>
+        <v>0.7082943364831135</v>
       </c>
       <c r="E6" t="n">
-        <v>2.392344497607656</v>
+        <v>23.44497607655502</v>
       </c>
       <c r="F6" t="n">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="G6" t="n">
-        <v>219</v>
+        <v>154</v>
       </c>
       <c r="H6" t="n">
-        <v>97.60765550239235</v>
+        <v>76.55502392344498</v>
       </c>
       <c r="I6" t="n">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -648,28 +648,28 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1846411483253587</v>
+        <v>1.315406698564593</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1420028456570982</v>
+        <v>0.8928911993515162</v>
       </c>
       <c r="E7" t="n">
-        <v>2.392344497607656</v>
+        <v>28.4688995215311</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="G7" t="n">
-        <v>225</v>
+        <v>143</v>
       </c>
       <c r="H7" t="n">
-        <v>97.60765550239235</v>
+        <v>71.5311004784689</v>
       </c>
       <c r="I7" t="n">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -680,28 +680,28 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2345933014354066</v>
+        <v>1.502488038277512</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1793197157397014</v>
+        <v>1.023896410757733</v>
       </c>
       <c r="E8" t="n">
-        <v>2.392344497607656</v>
+        <v>29.66507177033493</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="G8" t="n">
-        <v>229</v>
+        <v>141</v>
       </c>
       <c r="H8" t="n">
-        <v>97.60765550239235</v>
+        <v>70.33492822966507</v>
       </c>
       <c r="I8" t="n">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -712,28 +712,28 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.3046650717703349</v>
+        <v>1.814617224880383</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.2317560291278652</v>
+        <v>1.232201947360047</v>
       </c>
       <c r="E9" t="n">
-        <v>2.392344497607656</v>
+        <v>31.10047846889952</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="G9" t="n">
-        <v>227</v>
+        <v>130</v>
       </c>
       <c r="H9" t="n">
-        <v>97.60765550239235</v>
+        <v>68.89952153110048</v>
       </c>
       <c r="I9" t="n">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -744,28 +744,28 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.3680861244019137</v>
+        <v>2.097081339712919</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.2792866830784995</v>
+        <v>1.421294048385782</v>
       </c>
       <c r="E10" t="n">
-        <v>2.392344497607656</v>
+        <v>32.05741626794259</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="G10" t="n">
-        <v>227</v>
+        <v>128</v>
       </c>
       <c r="H10" t="n">
-        <v>97.60765550239235</v>
+        <v>67.94258373205741</v>
       </c>
       <c r="I10" t="n">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -776,28 +776,28 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.4098325358851673</v>
+        <v>2.713373205741627</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.3142652126834957</v>
+        <v>1.839049171340611</v>
       </c>
       <c r="E11" t="n">
-        <v>2.392344497607656</v>
+        <v>35.88516746411483</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="G11" t="n">
-        <v>234</v>
+        <v>120</v>
       </c>
       <c r="H11" t="n">
-        <v>97.60765550239235</v>
+        <v>64.11483253588517</v>
       </c>
       <c r="I11" t="n">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
@@ -808,28 +808,28 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.4111961722488036</v>
+        <v>3.003301435406698</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.3161788498587512</v>
+        <v>2.031742916192805</v>
       </c>
       <c r="E12" t="n">
-        <v>2.392344497607656</v>
+        <v>37.79904306220095</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="G12" t="n">
-        <v>231</v>
+        <v>110</v>
       </c>
       <c r="H12" t="n">
-        <v>97.60765550239235</v>
+        <v>62.20095693779905</v>
       </c>
       <c r="I12" t="n">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -840,28 +840,28 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.3418899521531099</v>
+        <v>3.204712918660286</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.2729340249873621</v>
+        <v>2.165913500819647</v>
       </c>
       <c r="E13" t="n">
-        <v>2.631578947368421</v>
+        <v>38.75598086124402</v>
       </c>
       <c r="F13" t="n">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="G13" t="n">
-        <v>226</v>
+        <v>109</v>
       </c>
       <c r="H13" t="n">
-        <v>97.36842105263158</v>
+        <v>61.24401913875598</v>
       </c>
       <c r="I13" t="n">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -872,28 +872,28 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.3149282296650712</v>
+        <v>3.585933014354067</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.2624667877070079</v>
+        <v>2.388542040862367</v>
       </c>
       <c r="E14" t="n">
-        <v>2.631578947368421</v>
+        <v>41.38755980861244</v>
       </c>
       <c r="F14" t="n">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="G14" t="n">
-        <v>224</v>
+        <v>98</v>
       </c>
       <c r="H14" t="n">
-        <v>97.36842105263158</v>
+        <v>58.61244019138756</v>
       </c>
       <c r="I14" t="n">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
@@ -904,28 +904,28 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.3380382775119616</v>
+        <v>3.919186602870812</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.2919024800242929</v>
+        <v>2.606538375948726</v>
       </c>
       <c r="E15" t="n">
-        <v>2.392344497607656</v>
+        <v>42.3444976076555</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="G15" t="n">
-        <v>227</v>
+        <v>96</v>
       </c>
       <c r="H15" t="n">
-        <v>97.60765550239235</v>
+        <v>57.65550239234449</v>
       </c>
       <c r="I15" t="n">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -936,28 +936,28 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.2359090909090907</v>
+        <v>4.24078947368421</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.2299836867857181</v>
+        <v>2.817839740579124</v>
       </c>
       <c r="E16" t="n">
-        <v>2.631578947368421</v>
+        <v>41.38755980861244</v>
       </c>
       <c r="F16" t="n">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="G16" t="n">
-        <v>228</v>
+        <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>97.36842105263158</v>
+        <v>58.61244019138756</v>
       </c>
       <c r="I16" t="n">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17">
@@ -968,28 +968,28 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.1884210526315789</v>
+        <v>4.663779904306219</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.2067839437284719</v>
+        <v>3.086060060181263</v>
       </c>
       <c r="E17" t="n">
-        <v>2.631578947368421</v>
+        <v>41.62679425837321</v>
       </c>
       <c r="F17" t="n">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="G17" t="n">
-        <v>232</v>
+        <v>98</v>
       </c>
       <c r="H17" t="n">
-        <v>97.36842105263158</v>
+        <v>58.3732057416268</v>
       </c>
       <c r="I17" t="n">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -1000,28 +1000,28 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.1285167464114831</v>
+        <v>4.876172248803827</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.1759593809572157</v>
+        <v>3.228117051049661</v>
       </c>
       <c r="E18" t="n">
-        <v>2.870813397129186</v>
+        <v>42.10526315789473</v>
       </c>
       <c r="F18" t="n">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="G18" t="n">
-        <v>228</v>
+        <v>97</v>
       </c>
       <c r="H18" t="n">
-        <v>97.1291866028708</v>
+        <v>57.89473684210527</v>
       </c>
       <c r="I18" t="n">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
@@ -1032,28 +1032,28 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.05009569377990444</v>
+        <v>5.196411483253589</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.1297108956965362</v>
+        <v>3.426923086192372</v>
       </c>
       <c r="E19" t="n">
-        <v>3.110047846889952</v>
+        <v>43.54066985645933</v>
       </c>
       <c r="F19" t="n">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="G19" t="n">
-        <v>221</v>
+        <v>86</v>
       </c>
       <c r="H19" t="n">
-        <v>96.88995215311004</v>
+        <v>56.45933014354066</v>
       </c>
       <c r="I19" t="n">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -1064,28 +1064,28 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.08909090909090857</v>
+        <v>5.133205741626794</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.1692617793441476</v>
+        <v>3.39279386790377</v>
       </c>
       <c r="E20" t="n">
-        <v>2.631578947368421</v>
+        <v>43.54066985645933</v>
       </c>
       <c r="F20" t="n">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>226</v>
+        <v>93</v>
       </c>
       <c r="H20" t="n">
-        <v>97.36842105263158</v>
+        <v>56.45933014354066</v>
       </c>
       <c r="I20" t="n">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -1096,28 +1096,28 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.02112440191387569</v>
+        <v>5.593133971291866</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1018214395263991</v>
+        <v>3.663526973884771</v>
       </c>
       <c r="E21" t="n">
-        <v>2.631578947368421</v>
+        <v>48.5645933014354</v>
       </c>
       <c r="F21" t="n">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="G21" t="n">
-        <v>221</v>
+        <v>77</v>
       </c>
       <c r="H21" t="n">
-        <v>97.36842105263158</v>
+        <v>51.43540669856459</v>
       </c>
       <c r="I21" t="n">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22">
@@ -1128,28 +1128,28 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.07423444976076549</v>
+        <v>6.05145933014354</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.0785708747575703</v>
+        <v>3.954705005193296</v>
       </c>
       <c r="E22" t="n">
-        <v>2.631578947368421</v>
+        <v>50.23923444976076</v>
       </c>
       <c r="F22" t="n">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="G22" t="n">
-        <v>218</v>
+        <v>68</v>
       </c>
       <c r="H22" t="n">
-        <v>97.36842105263158</v>
+        <v>49.76076555023923</v>
       </c>
       <c r="I22" t="n">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23">
@@ -1160,28 +1160,28 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1664114832535886</v>
+        <v>6.158373205741626</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.02691903917738865</v>
+        <v>4.012263295260095</v>
       </c>
       <c r="E23" t="n">
-        <v>2.870813397129186</v>
+        <v>51.43540669856459</v>
       </c>
       <c r="F23" t="n">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="G23" t="n">
-        <v>218</v>
+        <v>66</v>
       </c>
       <c r="H23" t="n">
-        <v>97.1291866028708</v>
+        <v>48.5645933014354</v>
       </c>
       <c r="I23" t="n">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
@@ -1192,28 +1192,28 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1599282296650718</v>
+        <v>6.615191387559808</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.04638049334815116</v>
+        <v>4.306524191231715</v>
       </c>
       <c r="E24" t="n">
-        <v>2.870813397129186</v>
+        <v>51.19617224880383</v>
       </c>
       <c r="F24" t="n">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="G24" t="n">
-        <v>218</v>
+        <v>65</v>
       </c>
       <c r="H24" t="n">
-        <v>97.1291866028708</v>
+        <v>48.80382775119617</v>
       </c>
       <c r="I24" t="n">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25">
@@ -1224,28 +1224,28 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.2031339712918659</v>
+        <v>6.837966507177033</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.02783957354166567</v>
+        <v>4.446525347018907</v>
       </c>
       <c r="E25" t="n">
-        <v>2.870813397129186</v>
+        <v>53.58851674641149</v>
       </c>
       <c r="F25" t="n">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="G25" t="n">
-        <v>218</v>
+        <v>60</v>
       </c>
       <c r="H25" t="n">
-        <v>97.1291866028708</v>
+        <v>46.41148325358851</v>
       </c>
       <c r="I25" t="n">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26">
@@ -1256,28 +1256,28 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2394019138755979</v>
+        <v>6.85366028708134</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.01436482640085407</v>
+        <v>4.440754812964752</v>
       </c>
       <c r="E26" t="n">
-        <v>2.870813397129186</v>
+        <v>54.54545454545454</v>
       </c>
       <c r="F26" t="n">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="G26" t="n">
-        <v>218</v>
+        <v>60</v>
       </c>
       <c r="H26" t="n">
-        <v>97.1291866028708</v>
+        <v>45.45454545454545</v>
       </c>
       <c r="I26" t="n">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27">
@@ -1288,28 +1288,28 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.2902153110047845</v>
+        <v>7.149784688995216</v>
       </c>
       <c r="D27" t="n">
-        <v>0.007441974097589462</v>
+        <v>4.628015129230259</v>
       </c>
       <c r="E27" t="n">
-        <v>2.870813397129186</v>
+        <v>54.78468899521531</v>
       </c>
       <c r="F27" t="n">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="G27" t="n">
-        <v>223</v>
+        <v>63</v>
       </c>
       <c r="H27" t="n">
-        <v>97.1291866028708</v>
+        <v>45.21531100478469</v>
       </c>
       <c r="I27" t="n">
-        <v>183</v>
+        <v>126</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28">
@@ -1320,28 +1320,28 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2727990430622012</v>
+        <v>7.449545454545454</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.0164382415315634</v>
+        <v>4.818476433806615</v>
       </c>
       <c r="E28" t="n">
-        <v>2.631578947368421</v>
+        <v>54.78468899521531</v>
       </c>
       <c r="F28" t="n">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="G28" t="n">
-        <v>221</v>
+        <v>61</v>
       </c>
       <c r="H28" t="n">
-        <v>97.36842105263158</v>
+        <v>45.21531100478469</v>
       </c>
       <c r="I28" t="n">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29">
@@ -1352,28 +1352,28 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.306578947368421</v>
+        <v>7.599784688995215</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.002374194467008674</v>
+        <v>4.908420976319418</v>
       </c>
       <c r="E29" t="n">
-        <v>2.631578947368421</v>
+        <v>55.26315789473685</v>
       </c>
       <c r="F29" t="n">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="G29" t="n">
-        <v>219</v>
+        <v>59</v>
       </c>
       <c r="H29" t="n">
-        <v>97.36842105263158</v>
+        <v>44.73684210526316</v>
       </c>
       <c r="I29" t="n">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30">
@@ -1384,28 +1384,28 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.4283014354066985</v>
+        <v>8.050454545454546</v>
       </c>
       <c r="D30" t="n">
-        <v>0.07700940277087345</v>
+        <v>5.203545928101089</v>
       </c>
       <c r="E30" t="n">
-        <v>2.870813397129186</v>
+        <v>54.30622009569378</v>
       </c>
       <c r="F30" t="n">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="G30" t="n">
-        <v>222</v>
+        <v>62</v>
       </c>
       <c r="H30" t="n">
-        <v>97.1291866028708</v>
+        <v>45.69377990430622</v>
       </c>
       <c r="I30" t="n">
-        <v>184</v>
+        <v>129</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31">
@@ -1416,28 +1416,28 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7636363636363638</v>
+        <v>8.362057416267943</v>
       </c>
       <c r="D31" t="n">
-        <v>0.312339264140883</v>
+        <v>5.394728301434532</v>
       </c>
       <c r="E31" t="n">
-        <v>3.349282296650718</v>
+        <v>55.26315789473685</v>
       </c>
       <c r="F31" t="n">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="G31" t="n">
-        <v>217</v>
+        <v>55</v>
       </c>
       <c r="H31" t="n">
-        <v>96.65071770334929</v>
+        <v>44.73684210526316</v>
       </c>
       <c r="I31" t="n">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
@@ -1448,28 +1448,28 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.6140191387559808</v>
+        <v>8.26645933014354</v>
       </c>
       <c r="D32" t="n">
-        <v>0.195321312326936</v>
+        <v>5.333968872756818</v>
       </c>
       <c r="E32" t="n">
-        <v>3.110047846889952</v>
+        <v>55.50239234449761</v>
       </c>
       <c r="F32" t="n">
-        <v>13</v>
+        <v>180</v>
       </c>
       <c r="G32" t="n">
-        <v>219</v>
+        <v>52</v>
       </c>
       <c r="H32" t="n">
-        <v>96.88995215311004</v>
+        <v>44.49760765550239</v>
       </c>
       <c r="I32" t="n">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33">
@@ -1480,28 +1480,28 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.782751196172249</v>
+        <v>8.514665071770334</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3121763328608665</v>
+        <v>5.496651462661533</v>
       </c>
       <c r="E33" t="n">
-        <v>3.349282296650718</v>
+        <v>55.74162679425837</v>
       </c>
       <c r="F33" t="n">
-        <v>14</v>
+        <v>179</v>
       </c>
       <c r="G33" t="n">
-        <v>218</v>
+        <v>53</v>
       </c>
       <c r="H33" t="n">
-        <v>96.65071770334929</v>
+        <v>44.25837320574163</v>
       </c>
       <c r="I33" t="n">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34">
@@ -1512,28 +1512,28 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8181100478468895</v>
+        <v>8.731842105263157</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3330358282729521</v>
+        <v>5.631304600543934</v>
       </c>
       <c r="E34" t="n">
-        <v>3.349282296650718</v>
+        <v>55.98086124401915</v>
       </c>
       <c r="F34" t="n">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="G34" t="n">
-        <v>221</v>
+        <v>58</v>
       </c>
       <c r="H34" t="n">
-        <v>96.65071770334929</v>
+        <v>44.01913875598086</v>
       </c>
       <c r="I34" t="n">
-        <v>183</v>
+        <v>126</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35">
@@ -1544,28 +1544,28 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>0.8094736842105261</v>
+        <v>8.563827751196174</v>
       </c>
       <c r="D35" t="n">
-        <v>0.3211762594209814</v>
+        <v>5.508881903540097</v>
       </c>
       <c r="E35" t="n">
-        <v>3.349282296650718</v>
+        <v>57.41626794258373</v>
       </c>
       <c r="F35" t="n">
-        <v>14</v>
+        <v>179</v>
       </c>
       <c r="G35" t="n">
-        <v>216</v>
+        <v>51</v>
       </c>
       <c r="H35" t="n">
-        <v>96.65071770334929</v>
+        <v>42.58373205741627</v>
       </c>
       <c r="I35" t="n">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36">
@@ -1576,28 +1576,28 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>0.8239712918660278</v>
+        <v>8.815023923444974</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3230192720283349</v>
+        <v>5.660838577125141</v>
       </c>
       <c r="E36" t="n">
-        <v>3.349282296650718</v>
+        <v>57.65550239234449</v>
       </c>
       <c r="F36" t="n">
-        <v>14</v>
+        <v>180</v>
       </c>
       <c r="G36" t="n">
-        <v>209</v>
+        <v>43</v>
       </c>
       <c r="H36" t="n">
-        <v>96.65071770334929</v>
+        <v>42.3444976076555</v>
       </c>
       <c r="I36" t="n">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37">
@@ -1608,28 +1608,28 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8247607655502392</v>
+        <v>8.984186602870814</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3128596547223554</v>
+        <v>5.762584966597216</v>
       </c>
       <c r="E37" t="n">
-        <v>3.349282296650718</v>
+        <v>57.89473684210527</v>
       </c>
       <c r="F37" t="n">
-        <v>14</v>
+        <v>181</v>
       </c>
       <c r="G37" t="n">
-        <v>209</v>
+        <v>42</v>
       </c>
       <c r="H37" t="n">
-        <v>96.65071770334929</v>
+        <v>42.10526315789473</v>
       </c>
       <c r="I37" t="n">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38">
@@ -1640,28 +1640,28 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>0.834354066985646</v>
+        <v>8.924306220095696</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3109948349325214</v>
+        <v>5.712136550941388</v>
       </c>
       <c r="E38" t="n">
-        <v>3.349282296650718</v>
+        <v>58.85167464114832</v>
       </c>
       <c r="F38" t="n">
-        <v>14</v>
+        <v>178</v>
       </c>
       <c r="G38" t="n">
-        <v>209</v>
+        <v>45</v>
       </c>
       <c r="H38" t="n">
-        <v>96.65071770334929</v>
+        <v>41.14832535885167</v>
       </c>
       <c r="I38" t="n">
-        <v>195</v>
+        <v>127</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39">
@@ -1672,28 +1672,28 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>0.8674162679425841</v>
+        <v>9.232057416267942</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3243923794825884</v>
+        <v>5.904057798117387</v>
       </c>
       <c r="E39" t="n">
-        <v>3.349282296650718</v>
+        <v>58.85167464114832</v>
       </c>
       <c r="F39" t="n">
-        <v>14</v>
+        <v>179</v>
       </c>
       <c r="G39" t="n">
-        <v>211</v>
+        <v>46</v>
       </c>
       <c r="H39" t="n">
-        <v>96.65071770334929</v>
+        <v>41.14832535885167</v>
       </c>
       <c r="I39" t="n">
-        <v>193</v>
+        <v>126</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40">
@@ -1704,28 +1704,28 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>0.5980382775119623</v>
+        <v>9.537177033492824</v>
       </c>
       <c r="D40" t="n">
-        <v>0.1185024519848346</v>
+        <v>6.092160819912343</v>
       </c>
       <c r="E40" t="n">
-        <v>2.870813397129186</v>
+        <v>58.85167464114832</v>
       </c>
       <c r="F40" t="n">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="G40" t="n">
-        <v>215</v>
+        <v>45</v>
       </c>
       <c r="H40" t="n">
-        <v>97.1291866028708</v>
+        <v>41.14832535885167</v>
       </c>
       <c r="I40" t="n">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41">
@@ -1736,28 +1736,28 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>0.6805023923444972</v>
+        <v>9.647488038277512</v>
       </c>
       <c r="D41" t="n">
-        <v>0.1744338326890667</v>
+        <v>6.163845027204264</v>
       </c>
       <c r="E41" t="n">
-        <v>2.870813397129186</v>
+        <v>58.85167464114832</v>
       </c>
       <c r="F41" t="n">
-        <v>12</v>
+        <v>181</v>
       </c>
       <c r="G41" t="n">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="H41" t="n">
-        <v>97.1291866028708</v>
+        <v>41.14832535885167</v>
       </c>
       <c r="I41" t="n">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42">
@@ -1768,28 +1768,28 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9904066985645933</v>
+        <v>9.858971291866029</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3951383569170053</v>
+        <v>6.295872776173317</v>
       </c>
       <c r="E42" t="n">
-        <v>3.349282296650718</v>
+        <v>58.85167464114832</v>
       </c>
       <c r="F42" t="n">
-        <v>14</v>
+        <v>183</v>
       </c>
       <c r="G42" t="n">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="H42" t="n">
-        <v>96.65071770334929</v>
+        <v>41.14832535885167</v>
       </c>
       <c r="I42" t="n">
-        <v>194</v>
+        <v>131</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43">
@@ -1800,28 +1800,28 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>0.948181818181818</v>
+        <v>9.98023923444976</v>
       </c>
       <c r="D43" t="n">
-        <v>0.360465741309228</v>
+        <v>6.369794443344373</v>
       </c>
       <c r="E43" t="n">
-        <v>3.349282296650718</v>
+        <v>59.33014354066985</v>
       </c>
       <c r="F43" t="n">
-        <v>14</v>
+        <v>181</v>
       </c>
       <c r="G43" t="n">
-        <v>200</v>
+        <v>33</v>
       </c>
       <c r="H43" t="n">
-        <v>96.65071770334929</v>
+        <v>40.66985645933015</v>
       </c>
       <c r="I43" t="n">
-        <v>204</v>
+        <v>137</v>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44">
@@ -1832,28 +1832,28 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8921531100478465</v>
+        <v>10.018995215311</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3145449612536612</v>
+        <v>6.396654138085872</v>
       </c>
       <c r="E44" t="n">
-        <v>3.349282296650718</v>
+        <v>59.56937799043062</v>
       </c>
       <c r="F44" t="n">
-        <v>14</v>
+        <v>182</v>
       </c>
       <c r="G44" t="n">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="H44" t="n">
-        <v>96.65071770334929</v>
+        <v>40.43062200956938</v>
       </c>
       <c r="I44" t="n">
-        <v>209</v>
+        <v>142</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45">
@@ -1864,28 +1864,28 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>0.9850717703349282</v>
+        <v>10.28382775119617</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3808977833572055</v>
+        <v>6.56013598467662</v>
       </c>
       <c r="E45" t="n">
-        <v>3.588516746411483</v>
+        <v>59.33014354066985</v>
       </c>
       <c r="F45" t="n">
-        <v>15</v>
+        <v>182</v>
       </c>
       <c r="G45" t="n">
-        <v>194</v>
+        <v>27</v>
       </c>
       <c r="H45" t="n">
-        <v>96.41148325358851</v>
+        <v>40.66985645933015</v>
       </c>
       <c r="I45" t="n">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="J45" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46">
@@ -1896,28 +1896,28 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>1.375645933014354</v>
+        <v>10.30980861244019</v>
       </c>
       <c r="D46" t="n">
-        <v>0.672237841204643</v>
+        <v>6.578475810852681</v>
       </c>
       <c r="E46" t="n">
-        <v>4.784688995215311</v>
+        <v>59.33014354066985</v>
       </c>
       <c r="F46" t="n">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="G46" t="n">
-        <v>186</v>
+        <v>27</v>
       </c>
       <c r="H46" t="n">
-        <v>95.21531100478468</v>
+        <v>40.66985645933015</v>
       </c>
       <c r="I46" t="n">
-        <v>212</v>
+        <v>143</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
@@ -1928,28 +1928,28 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9161004784688981</v>
+        <v>10.42624401913876</v>
       </c>
       <c r="D47" t="n">
-        <v>0.32400645269741</v>
+        <v>6.645886096100874</v>
       </c>
       <c r="E47" t="n">
-        <v>3.827751196172249</v>
+        <v>59.80861244019139</v>
       </c>
       <c r="F47" t="n">
-        <v>16</v>
+        <v>178</v>
       </c>
       <c r="G47" t="n">
-        <v>190</v>
+        <v>28</v>
       </c>
       <c r="H47" t="n">
-        <v>96.17224880382776</v>
+        <v>40.19138755980861</v>
       </c>
       <c r="I47" t="n">
-        <v>212</v>
+        <v>140</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48">
@@ -1960,28 +1960,28 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>1.119401913875598</v>
+        <v>10.03275119617225</v>
       </c>
       <c r="D48" t="n">
-        <v>0.4778439522711521</v>
+        <v>6.404880396094057</v>
       </c>
       <c r="E48" t="n">
-        <v>4.545454545454546</v>
+        <v>60.76555023923444</v>
       </c>
       <c r="F48" t="n">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="G48" t="n">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="H48" t="n">
-        <v>95.45454545454545</v>
+        <v>39.23444976076555</v>
       </c>
       <c r="I48" t="n">
-        <v>209</v>
+        <v>133</v>
       </c>
       <c r="J48" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49">
@@ -1992,28 +1992,28 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8395693779904302</v>
+        <v>10.07483253588517</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2682784044525934</v>
+        <v>6.432083855934335</v>
       </c>
       <c r="E49" t="n">
-        <v>4.066985645933014</v>
+        <v>61.00478468899522</v>
       </c>
       <c r="F49" t="n">
-        <v>17</v>
+        <v>177</v>
       </c>
       <c r="G49" t="n">
-        <v>193</v>
+        <v>33</v>
       </c>
       <c r="H49" t="n">
-        <v>95.93301435406698</v>
+        <v>38.99521531100478</v>
       </c>
       <c r="I49" t="n">
-        <v>208</v>
+        <v>130</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50">
@@ -2024,28 +2024,28 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.874138755980861</v>
+        <v>10.5638995215311</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2837022550496604</v>
+        <v>6.731631500247688</v>
       </c>
       <c r="E50" t="n">
-        <v>4.30622009569378</v>
+        <v>59.80861244019139</v>
       </c>
       <c r="F50" t="n">
-        <v>18</v>
+        <v>181</v>
       </c>
       <c r="G50" t="n">
-        <v>195</v>
+        <v>32</v>
       </c>
       <c r="H50" t="n">
-        <v>95.69377990430623</v>
+        <v>40.19138755980861</v>
       </c>
       <c r="I50" t="n">
-        <v>205</v>
+        <v>136</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51">
@@ -2056,28 +2056,28 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>1.20988038277512</v>
+        <v>10.59849282296651</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5263583783058757</v>
+        <v>6.756588644176853</v>
       </c>
       <c r="E51" t="n">
-        <v>5.023923444976076</v>
+        <v>59.56937799043062</v>
       </c>
       <c r="F51" t="n">
-        <v>21</v>
+        <v>178</v>
       </c>
       <c r="G51" t="n">
-        <v>189</v>
+        <v>32</v>
       </c>
       <c r="H51" t="n">
-        <v>94.97607655502392</v>
+        <v>40.43062200956938</v>
       </c>
       <c r="I51" t="n">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52">
@@ -2088,28 +2088,28 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>1.204880382775119</v>
+        <v>10.71071770334928</v>
       </c>
       <c r="D52" t="n">
-        <v>0.5143402239687545</v>
+        <v>6.825341229638199</v>
       </c>
       <c r="E52" t="n">
-        <v>5.023923444976076</v>
+        <v>60.04784688995215</v>
       </c>
       <c r="F52" t="n">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="G52" t="n">
-        <v>195</v>
+        <v>33</v>
       </c>
       <c r="H52" t="n">
-        <v>94.97607655502392</v>
+        <v>39.95215311004785</v>
       </c>
       <c r="I52" t="n">
-        <v>202</v>
+        <v>134</v>
       </c>
       <c r="J52" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53">
@@ -2120,28 +2120,28 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>1.497511961722488</v>
+        <v>10.85775119617225</v>
       </c>
       <c r="D53" t="n">
-        <v>0.7252012574068777</v>
+        <v>6.919086284887986</v>
       </c>
       <c r="E53" t="n">
-        <v>5.502392344497608</v>
+        <v>60.04784688995215</v>
       </c>
       <c r="F53" t="n">
-        <v>23</v>
+        <v>180</v>
       </c>
       <c r="G53" t="n">
-        <v>194</v>
+        <v>37</v>
       </c>
       <c r="H53" t="n">
-        <v>94.49760765550239</v>
+        <v>39.95215311004785</v>
       </c>
       <c r="I53" t="n">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="J53" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54">
@@ -2152,28 +2152,28 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>1.131674641148325</v>
+        <v>11.03129186602871</v>
       </c>
       <c r="D54" t="n">
-        <v>0.4475331865648925</v>
+        <v>7.027025783548828</v>
       </c>
       <c r="E54" t="n">
-        <v>5.023923444976076</v>
+        <v>59.80861244019139</v>
       </c>
       <c r="F54" t="n">
-        <v>21</v>
+        <v>181</v>
       </c>
       <c r="G54" t="n">
-        <v>196</v>
+        <v>36</v>
       </c>
       <c r="H54" t="n">
-        <v>94.97607655502392</v>
+        <v>40.19138755980861</v>
       </c>
       <c r="I54" t="n">
-        <v>201</v>
+        <v>132</v>
       </c>
       <c r="J54" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55">
@@ -2184,28 +2184,28 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9018181818181819</v>
+        <v>11.26162679425837</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2741866791913349</v>
+        <v>7.171535765741775</v>
       </c>
       <c r="E55" t="n">
-        <v>4.545454545454546</v>
+        <v>59.33014354066985</v>
       </c>
       <c r="F55" t="n">
-        <v>19</v>
+        <v>181</v>
       </c>
       <c r="G55" t="n">
-        <v>197</v>
+        <v>35</v>
       </c>
       <c r="H55" t="n">
-        <v>95.45454545454545</v>
+        <v>40.66985645933015</v>
       </c>
       <c r="I55" t="n">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56">
@@ -2216,28 +2216,28 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>1.301913875598085</v>
+        <v>11.3455023923445</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5650355279288908</v>
+        <v>7.226541056729024</v>
       </c>
       <c r="E56" t="n">
-        <v>5.263157894736842</v>
+        <v>59.56937799043062</v>
       </c>
       <c r="F56" t="n">
-        <v>22</v>
+        <v>180</v>
       </c>
       <c r="G56" t="n">
-        <v>192</v>
+        <v>34</v>
       </c>
       <c r="H56" t="n">
-        <v>94.73684210526315</v>
+        <v>40.43062200956938</v>
       </c>
       <c r="I56" t="n">
-        <v>204</v>
+        <v>135</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57">
@@ -2248,28 +2248,28 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>1.335334928229665</v>
+        <v>11.26528708133971</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5866664914079479</v>
+        <v>7.176376381626319</v>
       </c>
       <c r="E57" t="n">
-        <v>5.263157894736842</v>
+        <v>61.00478468899522</v>
       </c>
       <c r="F57" t="n">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="G57" t="n">
-        <v>193</v>
+        <v>32</v>
       </c>
       <c r="H57" t="n">
-        <v>94.73684210526315</v>
+        <v>38.99521531100478</v>
       </c>
       <c r="I57" t="n">
-        <v>203</v>
+        <v>131</v>
       </c>
       <c r="J57" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58">
@@ -2280,28 +2280,28 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>1.522607655502391</v>
+        <v>11.37514354066986</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7184281034407106</v>
+        <v>7.251566056975392</v>
       </c>
       <c r="E58" t="n">
-        <v>5.502392344497608</v>
+        <v>61.24401913875598</v>
       </c>
       <c r="F58" t="n">
-        <v>23</v>
+        <v>183</v>
       </c>
       <c r="G58" t="n">
-        <v>188</v>
+        <v>28</v>
       </c>
       <c r="H58" t="n">
-        <v>94.49760765550239</v>
+        <v>38.75598086124402</v>
       </c>
       <c r="I58" t="n">
-        <v>207</v>
+        <v>134</v>
       </c>
       <c r="J58" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59">
@@ -2312,28 +2312,28 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>1.511435406698564</v>
+        <v>11.42688995215311</v>
       </c>
       <c r="D59" t="n">
-        <v>0.7101354838229669</v>
+        <v>7.290320666273145</v>
       </c>
       <c r="E59" t="n">
-        <v>5.502392344497608</v>
+        <v>61.96172248803828</v>
       </c>
       <c r="F59" t="n">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="G59" t="n">
-        <v>187</v>
+        <v>29</v>
       </c>
       <c r="H59" t="n">
-        <v>94.49760765550239</v>
+        <v>38.03827751196172</v>
       </c>
       <c r="I59" t="n">
-        <v>208</v>
+        <v>130</v>
       </c>
       <c r="J59" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60">
@@ -2344,28 +2344,28 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>1.638564593301435</v>
+        <v>11.50502392344498</v>
       </c>
       <c r="D60" t="n">
-        <v>0.8014162791525022</v>
+        <v>7.349589402709297</v>
       </c>
       <c r="E60" t="n">
-        <v>5.741626794258373</v>
+        <v>61.72248803827751</v>
       </c>
       <c r="F60" t="n">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="G60" t="n">
-        <v>183</v>
+        <v>29</v>
       </c>
       <c r="H60" t="n">
-        <v>94.25837320574163</v>
+        <v>38.27751196172249</v>
       </c>
       <c r="I60" t="n">
-        <v>211</v>
+        <v>131</v>
       </c>
       <c r="J60" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61">
@@ -2376,28 +2376,28 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>1.645574162679426</v>
+        <v>11.58729665071771</v>
       </c>
       <c r="D61" t="n">
-        <v>0.8056950030925072</v>
+        <v>7.40866432535636</v>
       </c>
       <c r="E61" t="n">
-        <v>5.741626794258373</v>
+        <v>61.96172248803828</v>
       </c>
       <c r="F61" t="n">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="G61" t="n">
-        <v>184</v>
+        <v>30</v>
       </c>
       <c r="H61" t="n">
-        <v>94.25837320574163</v>
+        <v>38.03827751196172</v>
       </c>
       <c r="I61" t="n">
-        <v>210</v>
+        <v>129</v>
       </c>
       <c r="J61" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62">
@@ -2408,28 +2408,28 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>2.016698564593301</v>
+        <v>11.6122966507177</v>
       </c>
       <c r="D62" t="n">
-        <v>1.086682175952071</v>
+        <v>7.432786242171153</v>
       </c>
       <c r="E62" t="n">
-        <v>6.45933014354067</v>
+        <v>61.24401913875598</v>
       </c>
       <c r="F62" t="n">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G62" t="n">
-        <v>179</v>
+        <v>29</v>
       </c>
       <c r="H62" t="n">
-        <v>93.54066985645933</v>
+        <v>38.75598086124402</v>
       </c>
       <c r="I62" t="n">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="J62" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63">
@@ -2440,28 +2440,28 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>1.987918660287083</v>
+        <v>11.59074162679426</v>
       </c>
       <c r="D63" t="n">
-        <v>1.064005347911448</v>
+        <v>7.430348275819493</v>
       </c>
       <c r="E63" t="n">
-        <v>6.45933014354067</v>
+        <v>61.24401913875598</v>
       </c>
       <c r="F63" t="n">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G63" t="n">
-        <v>178</v>
+        <v>26</v>
       </c>
       <c r="H63" t="n">
-        <v>93.54066985645933</v>
+        <v>38.75598086124402</v>
       </c>
       <c r="I63" t="n">
-        <v>213</v>
+        <v>136</v>
       </c>
       <c r="J63" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64">
@@ -2472,28 +2472,28 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>1.890406698564592</v>
+        <v>11.50523923444976</v>
       </c>
       <c r="D64" t="n">
-        <v>0.9924649719217159</v>
+        <v>7.381182584395757</v>
       </c>
       <c r="E64" t="n">
-        <v>6.45933014354067</v>
+        <v>61.48325358851675</v>
       </c>
       <c r="F64" t="n">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="G64" t="n">
-        <v>176</v>
+        <v>23</v>
       </c>
       <c r="H64" t="n">
-        <v>93.54066985645933</v>
+        <v>38.51674641148325</v>
       </c>
       <c r="I64" t="n">
-        <v>215</v>
+        <v>138</v>
       </c>
       <c r="J64" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65">
@@ -2504,28 +2504,28 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>1.807775119617224</v>
+        <v>11.63227272727273</v>
       </c>
       <c r="D65" t="n">
-        <v>0.9314295134749471</v>
+        <v>7.462989928130844</v>
       </c>
       <c r="E65" t="n">
-        <v>6.45933014354067</v>
+        <v>61.72248803827751</v>
       </c>
       <c r="F65" t="n">
-        <v>27</v>
+        <v>182</v>
       </c>
       <c r="G65" t="n">
-        <v>177</v>
+        <v>22</v>
       </c>
       <c r="H65" t="n">
-        <v>93.54066985645933</v>
+        <v>38.27751196172249</v>
       </c>
       <c r="I65" t="n">
-        <v>214</v>
+        <v>138</v>
       </c>
       <c r="J65" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66">
@@ -2536,28 +2536,28 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>1.791555023923445</v>
+        <v>11.63973684210526</v>
       </c>
       <c r="D66" t="n">
-        <v>0.916438814540498</v>
+        <v>7.476108100343809</v>
       </c>
       <c r="E66" t="n">
-        <v>6.45933014354067</v>
+        <v>61.00478468899522</v>
       </c>
       <c r="F66" t="n">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G66" t="n">
-        <v>176</v>
+        <v>24</v>
       </c>
       <c r="H66" t="n">
-        <v>93.54066985645933</v>
+        <v>38.99521531100478</v>
       </c>
       <c r="I66" t="n">
-        <v>215</v>
+        <v>139</v>
       </c>
       <c r="J66" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67">
@@ -2568,28 +2568,28 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>1.809114832535884</v>
+        <v>11.73322966507177</v>
       </c>
       <c r="D67" t="n">
-        <v>0.9246119554835593</v>
+        <v>7.534023690993785</v>
       </c>
       <c r="E67" t="n">
-        <v>6.698564593301436</v>
+        <v>61.48325358851675</v>
       </c>
       <c r="F67" t="n">
-        <v>28</v>
+        <v>181</v>
       </c>
       <c r="G67" t="n">
-        <v>177</v>
+        <v>24</v>
       </c>
       <c r="H67" t="n">
-        <v>93.30143540669856</v>
+        <v>38.51674641148325</v>
       </c>
       <c r="I67" t="n">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="J67" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68">
@@ -2600,28 +2600,28 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>1.764976076555023</v>
+        <v>11.88105263157895</v>
       </c>
       <c r="D68" t="n">
-        <v>0.8885105189485148</v>
+        <v>7.631006642042023</v>
       </c>
       <c r="E68" t="n">
-        <v>6.45933014354067</v>
+        <v>61.48325358851675</v>
       </c>
       <c r="F68" t="n">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="G68" t="n">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="H68" t="n">
-        <v>93.54066985645933</v>
+        <v>38.51674641148325</v>
       </c>
       <c r="I68" t="n">
-        <v>212</v>
+        <v>139</v>
       </c>
       <c r="J68" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69">
@@ -2632,28 +2632,28 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>1.863875598086123</v>
+        <v>12.44143540669856</v>
       </c>
       <c r="D69" t="n">
-        <v>0.9623245240489057</v>
+        <v>7.978297787812161</v>
       </c>
       <c r="E69" t="n">
-        <v>6.937799043062201</v>
+        <v>60.04784688995215</v>
       </c>
       <c r="F69" t="n">
-        <v>29</v>
+        <v>184</v>
       </c>
       <c r="G69" t="n">
-        <v>176</v>
+        <v>21</v>
       </c>
       <c r="H69" t="n">
-        <v>93.0622009569378</v>
+        <v>39.95215311004785</v>
       </c>
       <c r="I69" t="n">
-        <v>213</v>
+        <v>146</v>
       </c>
       <c r="J69" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70">
@@ -2664,28 +2664,28 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>1.90035885167464</v>
+        <v>12.50064593301435</v>
       </c>
       <c r="D70" t="n">
-        <v>0.989530218955245</v>
+        <v>8.012369465164079</v>
       </c>
       <c r="E70" t="n">
-        <v>7.177033492822966</v>
+        <v>60.28708133971292</v>
       </c>
       <c r="F70" t="n">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="G70" t="n">
-        <v>183</v>
+        <v>22</v>
       </c>
       <c r="H70" t="n">
-        <v>92.82296650717703</v>
+        <v>39.71291866028708</v>
       </c>
       <c r="I70" t="n">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="J70" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71">
@@ -2696,28 +2696,28 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>1.810574162679426</v>
+        <v>12.58593301435407</v>
       </c>
       <c r="D71" t="n">
-        <v>0.9188800322855563</v>
+        <v>8.063374618598882</v>
       </c>
       <c r="E71" t="n">
-        <v>7.416267942583731</v>
+        <v>60.28708133971292</v>
       </c>
       <c r="F71" t="n">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="G71" t="n">
-        <v>183</v>
+        <v>22</v>
       </c>
       <c r="H71" t="n">
-        <v>92.58373205741627</v>
+        <v>39.71291866028708</v>
       </c>
       <c r="I71" t="n">
-        <v>204</v>
+        <v>144</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72">
@@ -2728,28 +2728,28 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>1.72712918660287</v>
+        <v>13.35784688995215</v>
       </c>
       <c r="D72" t="n">
-        <v>0.8546765060306886</v>
+        <v>8.561769727253337</v>
       </c>
       <c r="E72" t="n">
-        <v>7.416267942583731</v>
+        <v>58.61244019138756</v>
       </c>
       <c r="F72" t="n">
-        <v>30</v>
+        <v>199</v>
       </c>
       <c r="G72" t="n">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="H72" t="n">
-        <v>92.58373205741627</v>
+        <v>41.38755980861244</v>
       </c>
       <c r="I72" t="n">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="J72" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73">
@@ -2760,28 +2760,28 @@
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>1.701411483253588</v>
+        <v>13.34571770334928</v>
       </c>
       <c r="D73" t="n">
-        <v>0.8310854687216814</v>
+        <v>8.555767191566941</v>
       </c>
       <c r="E73" t="n">
-        <v>7.416267942583731</v>
+        <v>58.61244019138756</v>
       </c>
       <c r="F73" t="n">
-        <v>30</v>
+        <v>197</v>
       </c>
       <c r="G73" t="n">
-        <v>186</v>
+        <v>19</v>
       </c>
       <c r="H73" t="n">
-        <v>92.58373205741627</v>
+        <v>41.38755980861244</v>
       </c>
       <c r="I73" t="n">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="J73" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74">
@@ -2792,28 +2792,28 @@
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>1.97078947368421</v>
+        <v>13.80533492822967</v>
       </c>
       <c r="D74" t="n">
-        <v>1.022630447842766</v>
+        <v>8.857881779794113</v>
       </c>
       <c r="E74" t="n">
-        <v>8.133971291866029</v>
+        <v>57.65550239234449</v>
       </c>
       <c r="F74" t="n">
-        <v>32</v>
+        <v>198</v>
       </c>
       <c r="G74" t="n">
-        <v>186</v>
+        <v>20</v>
       </c>
       <c r="H74" t="n">
-        <v>91.86602870813397</v>
+        <v>42.3444976076555</v>
       </c>
       <c r="I74" t="n">
-        <v>198</v>
+        <v>157</v>
       </c>
       <c r="J74" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75">
@@ -2824,28 +2824,28 @@
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>1.858062200956938</v>
+        <v>13.62375598086125</v>
       </c>
       <c r="D75" t="n">
-        <v>0.9390655567346182</v>
+        <v>8.741663739403752</v>
       </c>
       <c r="E75" t="n">
-        <v>7.894736842105263</v>
+        <v>57.89473684210527</v>
       </c>
       <c r="F75" t="n">
-        <v>33</v>
+        <v>200</v>
       </c>
       <c r="G75" t="n">
-        <v>189</v>
+        <v>22</v>
       </c>
       <c r="H75" t="n">
-        <v>92.10526315789474</v>
+        <v>42.10526315789473</v>
       </c>
       <c r="I75" t="n">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="J75" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76">
@@ -2856,28 +2856,28 @@
         <v>75</v>
       </c>
       <c r="C76" t="n">
-        <v>1.896555023923445</v>
+        <v>14.04894736842106</v>
       </c>
       <c r="D76" t="n">
-        <v>0.9677078823136565</v>
+        <v>9.015246076214016</v>
       </c>
       <c r="E76" t="n">
-        <v>7.894736842105263</v>
+        <v>57.65550239234449</v>
       </c>
       <c r="F76" t="n">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="G76" t="n">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="H76" t="n">
-        <v>92.10526315789474</v>
+        <v>42.3444976076555</v>
       </c>
       <c r="I76" t="n">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="J76" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77">
@@ -2888,28 +2888,28 @@
         <v>76</v>
       </c>
       <c r="C77" t="n">
-        <v>1.788827751196172</v>
+        <v>14.11313397129187</v>
       </c>
       <c r="D77" t="n">
-        <v>0.88566632201249</v>
+        <v>9.061183571377308</v>
       </c>
       <c r="E77" t="n">
-        <v>7.894736842105263</v>
+        <v>57.65550239234449</v>
       </c>
       <c r="F77" t="n">
-        <v>33</v>
+        <v>202</v>
       </c>
       <c r="G77" t="n">
-        <v>197</v>
+        <v>28</v>
       </c>
       <c r="H77" t="n">
-        <v>92.10526315789474</v>
+        <v>42.3444976076555</v>
       </c>
       <c r="I77" t="n">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="J77" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78">
@@ -2920,28 +2920,28 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>1.853851674641148</v>
+        <v>14.20112440191387</v>
       </c>
       <c r="D78" t="n">
-        <v>0.9295221341453166</v>
+        <v>9.125159361176848</v>
       </c>
       <c r="E78" t="n">
-        <v>7.894736842105263</v>
+        <v>57.41626794258373</v>
       </c>
       <c r="F78" t="n">
-        <v>33</v>
+        <v>203</v>
       </c>
       <c r="G78" t="n">
-        <v>196</v>
+        <v>26</v>
       </c>
       <c r="H78" t="n">
-        <v>92.10526315789474</v>
+        <v>42.58373205741627</v>
       </c>
       <c r="I78" t="n">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="J78" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79">
@@ -2952,28 +2952,28 @@
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>1.888062200956937</v>
+        <v>14.3438995215311</v>
       </c>
       <c r="D79" t="n">
-        <v>0.950889914692467</v>
+        <v>9.232855581331654</v>
       </c>
       <c r="E79" t="n">
-        <v>7.894736842105263</v>
+        <v>56.69856459330143</v>
       </c>
       <c r="F79" t="n">
-        <v>33</v>
+        <v>196</v>
       </c>
       <c r="G79" t="n">
-        <v>189</v>
+        <v>26</v>
       </c>
       <c r="H79" t="n">
-        <v>92.10526315789474</v>
+        <v>43.30143540669857</v>
       </c>
       <c r="I79" t="n">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="J79" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80">
@@ -2984,28 +2984,28 @@
         <v>79</v>
       </c>
       <c r="C80" t="n">
-        <v>1.839545454545455</v>
+        <v>14.03700956937799</v>
       </c>
       <c r="D80" t="n">
-        <v>0.914921508956464</v>
+        <v>9.035683857182731</v>
       </c>
       <c r="E80" t="n">
-        <v>7.894736842105263</v>
+        <v>59.09090909090909</v>
       </c>
       <c r="F80" t="n">
-        <v>33</v>
+        <v>202</v>
       </c>
       <c r="G80" t="n">
-        <v>191</v>
+        <v>22</v>
       </c>
       <c r="H80" t="n">
-        <v>92.10526315789474</v>
+        <v>40.90909090909091</v>
       </c>
       <c r="I80" t="n">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="J80" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81">
@@ -3016,28 +3016,28 @@
         <v>80</v>
       </c>
       <c r="C81" t="n">
-        <v>1.812105263157895</v>
+        <v>14.87861244019139</v>
       </c>
       <c r="D81" t="n">
-        <v>0.8916354175830276</v>
+        <v>9.584333128549268</v>
       </c>
       <c r="E81" t="n">
-        <v>7.894736842105263</v>
+        <v>57.17703349282297</v>
       </c>
       <c r="F81" t="n">
-        <v>33</v>
+        <v>199</v>
       </c>
       <c r="G81" t="n">
-        <v>191</v>
+        <v>25</v>
       </c>
       <c r="H81" t="n">
-        <v>92.10526315789474</v>
+        <v>42.82296650717704</v>
       </c>
       <c r="I81" t="n">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="J81" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82">
@@ -3048,28 +3048,28 @@
         <v>81</v>
       </c>
       <c r="C82" t="n">
-        <v>1.925813397129187</v>
+        <v>14.83921052631579</v>
       </c>
       <c r="D82" t="n">
-        <v>0.9766265807432388</v>
+        <v>9.570964855890598</v>
       </c>
       <c r="E82" t="n">
-        <v>8.133971291866029</v>
+        <v>56.9377990430622</v>
       </c>
       <c r="F82" t="n">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="G82" t="n">
-        <v>190</v>
+        <v>24</v>
       </c>
       <c r="H82" t="n">
-        <v>91.86602870813397</v>
+        <v>43.0622009569378</v>
       </c>
       <c r="I82" t="n">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="J82" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83">
@@ -3080,28 +3080,28 @@
         <v>82</v>
       </c>
       <c r="C83" t="n">
-        <v>2.070430622009569</v>
+        <v>14.88942583732057</v>
       </c>
       <c r="D83" t="n">
-        <v>1.083270904297784</v>
+        <v>9.612769458508534</v>
       </c>
       <c r="E83" t="n">
-        <v>8.373205741626794</v>
+        <v>56.2200956937799</v>
       </c>
       <c r="F83" t="n">
-        <v>35</v>
+        <v>195</v>
       </c>
       <c r="G83" t="n">
-        <v>187</v>
+        <v>27</v>
       </c>
       <c r="H83" t="n">
-        <v>91.6267942583732</v>
+        <v>43.7799043062201</v>
       </c>
       <c r="I83" t="n">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="J83" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84">
@@ -3112,28 +3112,28 @@
         <v>83</v>
       </c>
       <c r="C84" t="n">
-        <v>2.299234449760766</v>
+        <v>14.8955023923445</v>
       </c>
       <c r="D84" t="n">
-        <v>1.247070537494187</v>
+        <v>9.624876508221865</v>
       </c>
       <c r="E84" t="n">
-        <v>8.612440191387559</v>
+        <v>56.69856459330143</v>
       </c>
       <c r="F84" t="n">
-        <v>36</v>
+        <v>194</v>
       </c>
       <c r="G84" t="n">
-        <v>185</v>
+        <v>27</v>
       </c>
       <c r="H84" t="n">
-        <v>91.38755980861244</v>
+        <v>43.30143540669857</v>
       </c>
       <c r="I84" t="n">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="J84" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85">
@@ -3144,28 +3144,28 @@
         <v>84</v>
       </c>
       <c r="C85" t="n">
-        <v>2.282081339712918</v>
+        <v>15.13480861244019</v>
       </c>
       <c r="D85" t="n">
-        <v>1.230895685446388</v>
+        <v>9.789908255045599</v>
       </c>
       <c r="E85" t="n">
-        <v>8.373205741626794</v>
+        <v>53.34928229665071</v>
       </c>
       <c r="F85" t="n">
-        <v>35</v>
+        <v>186</v>
       </c>
       <c r="G85" t="n">
-        <v>185</v>
+        <v>34</v>
       </c>
       <c r="H85" t="n">
-        <v>91.6267942583732</v>
+        <v>46.65071770334928</v>
       </c>
       <c r="I85" t="n">
-        <v>198</v>
+        <v>161</v>
       </c>
       <c r="J85" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86">
@@ -3176,28 +3176,28 @@
         <v>85</v>
       </c>
       <c r="C86" t="n">
-        <v>2.31177033492823</v>
+        <v>15.00837320574163</v>
       </c>
       <c r="D86" t="n">
-        <v>1.249590396111386</v>
+        <v>9.716752559742517</v>
       </c>
       <c r="E86" t="n">
-        <v>8.612440191387559</v>
+        <v>51.91387559808612</v>
       </c>
       <c r="F86" t="n">
-        <v>36</v>
+        <v>178</v>
       </c>
       <c r="G86" t="n">
-        <v>182</v>
+        <v>40</v>
       </c>
       <c r="H86" t="n">
-        <v>91.38755980861244</v>
+        <v>48.08612440191388</v>
       </c>
       <c r="I86" t="n">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="J86" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="87">
@@ -3208,28 +3208,28 @@
         <v>86</v>
       </c>
       <c r="C87" t="n">
-        <v>2.090885167464114</v>
+        <v>14.65906698564593</v>
       </c>
       <c r="D87" t="n">
-        <v>1.084221930128757</v>
+        <v>9.515805728549486</v>
       </c>
       <c r="E87" t="n">
-        <v>8.133971291866029</v>
+        <v>51.19617224880383</v>
       </c>
       <c r="F87" t="n">
-        <v>34</v>
+        <v>173</v>
       </c>
       <c r="G87" t="n">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="H87" t="n">
-        <v>91.86602870813397</v>
+        <v>48.80382775119617</v>
       </c>
       <c r="I87" t="n">
-        <v>202</v>
+        <v>161</v>
       </c>
       <c r="J87" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88">
@@ -3240,28 +3240,28 @@
         <v>87</v>
       </c>
       <c r="C88" t="n">
-        <v>2.366531100478467</v>
+        <v>14.61997607655502</v>
       </c>
       <c r="D88" t="n">
-        <v>1.288620630757688</v>
+        <v>9.49571801731874</v>
       </c>
       <c r="E88" t="n">
-        <v>8.851674641148326</v>
+        <v>51.43540669856459</v>
       </c>
       <c r="F88" t="n">
-        <v>36</v>
+        <v>177</v>
       </c>
       <c r="G88" t="n">
-        <v>183</v>
+        <v>42</v>
       </c>
       <c r="H88" t="n">
-        <v>91.14832535885168</v>
+        <v>48.5645933014354</v>
       </c>
       <c r="I88" t="n">
-        <v>198</v>
+        <v>161</v>
       </c>
       <c r="J88" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89">
@@ -3272,28 +3272,28 @@
         <v>88</v>
       </c>
       <c r="C89" t="n">
-        <v>2.360622009569378</v>
+        <v>13.99722488038278</v>
       </c>
       <c r="D89" t="n">
-        <v>1.282838376072405</v>
+        <v>9.121385597862458</v>
       </c>
       <c r="E89" t="n">
-        <v>8.851674641148326</v>
+        <v>53.34928229665071</v>
       </c>
       <c r="F89" t="n">
-        <v>36</v>
+        <v>172</v>
       </c>
       <c r="G89" t="n">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="H89" t="n">
-        <v>91.14832535885168</v>
+        <v>46.65071770334928</v>
       </c>
       <c r="I89" t="n">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="J89" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90">
@@ -3304,28 +3304,28 @@
         <v>89</v>
       </c>
       <c r="C90" t="n">
-        <v>2.387631578947367</v>
+        <v>13.86782296650718</v>
       </c>
       <c r="D90" t="n">
-        <v>1.299369264168272</v>
+        <v>9.044461862647449</v>
       </c>
       <c r="E90" t="n">
-        <v>8.851674641148326</v>
+        <v>53.58851674641149</v>
       </c>
       <c r="F90" t="n">
-        <v>35</v>
+        <v>170</v>
       </c>
       <c r="G90" t="n">
-        <v>183</v>
+        <v>48</v>
       </c>
       <c r="H90" t="n">
-        <v>91.14832535885168</v>
+        <v>46.41148325358851</v>
       </c>
       <c r="I90" t="n">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="J90" t="n">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91">
@@ -3336,28 +3336,28 @@
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>2.358373205741627</v>
+        <v>14.05062200956938</v>
       </c>
       <c r="D91" t="n">
-        <v>1.273790295442323</v>
+        <v>9.159932694559034</v>
       </c>
       <c r="E91" t="n">
-        <v>8.851674641148326</v>
+        <v>53.34928229665071</v>
       </c>
       <c r="F91" t="n">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="G91" t="n">
-        <v>186</v>
+        <v>47</v>
       </c>
       <c r="H91" t="n">
-        <v>91.14832535885168</v>
+        <v>46.65071770334928</v>
       </c>
       <c r="I91" t="n">
-        <v>195</v>
+        <v>148</v>
       </c>
       <c r="J91" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>